<commit_message>
Fim da aula de 13-11-24
</commit_message>
<xml_diff>
--- a/dados/saida.xlsx
+++ b/dados/saida.xlsx
@@ -1,32 +1,14 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
-  </bookViews>
-  <sheets>
-    <sheet name="NovaPlanilha" sheetId="1" state="visible" r:id="rId1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
-</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +19,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +27,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,85 +390,4 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Nome</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Idade</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Alice</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>25</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>alice@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>30</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>bob@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Carol</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>22</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>carol@example.com</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>